<commit_message>
feat: 新增 System.DateTime 相关断言方法。
BREAKING CHANGE: 增加了 .NET 6+ 支持。
</commit_message>
<xml_diff>
--- a/assets/Design/01 编码定义 (Codes).xlsx
+++ b/assets/Design/01 编码定义 (Codes).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>序号
 Index</t>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>参数值为 NULL 值，将使用 “ifNull”参数值替代，请关注。</t>
+  </si>
+  <si>
+    <t>参数 “{0}”超出了指定的范围。</t>
+  </si>
+  <si>
+    <t>参数 “{0}”超出了指定的范围 “{1}”。</t>
+  </si>
+  <si>
+    <t>参数超出了指定的范围。</t>
+  </si>
+  <si>
+    <t>参数超出了指定的范围 “{0}”。</t>
   </si>
 </sst>
 </file>
@@ -1307,18 +1319,18 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f t="shared" ref="C2:C10" si="0">_xlfn.SWITCH(B2,"Trace","T","Debug","D","Information","I","Warning","W","Error","E","Exception","X")</f>
+        <f t="shared" ref="C2:C11" si="0">_xlfn.SWITCH(B2,"Trace","T","Debug","D","Information","I","Warning","W","Error","E","Exception","X")</f>
         <v>X</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D10" si="1">"PL"&amp;C2&amp;RIGHT("0000"&amp;A2,4)</f>
+        <f t="shared" ref="D2:D11" si="1">"PL"&amp;C2&amp;RIGHT("0000"&amp;A2,4)</f>
         <v>PLX0001</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="4" t="str">
-        <f t="shared" ref="F2:F10" si="2">D2&amp;": "&amp;E2</f>
+        <f t="shared" ref="F2:F11" si="2">D2&amp;": "&amp;E2</f>
         <v>PLX0001: 应用程序抛出了一个未处理的异常。</v>
       </c>
     </row>
@@ -1514,39 +1526,111 @@
         <v>15</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f>_xlfn.SWITCH(B11,"Trace","T","Debug","D","Information","I","Warning","W","Error","E","Exception","X")</f>
+        <f t="shared" si="0"/>
         <v>D</v>
       </c>
       <c r="D11" s="3" t="str">
-        <f>"PL"&amp;C11&amp;RIGHT("0000"&amp;A11,4)</f>
+        <f t="shared" si="1"/>
         <v>PLD0010</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="4" t="str">
-        <f>D11&amp;": "&amp;E11</f>
+        <f t="shared" si="2"/>
         <v>PLD0010: 参数值为 NULL 值，将使用 “ifNull”参数值替代，请关注。</v>
       </c>
     </row>
-    <row r="12" customHeight="1" spans="1:1">
+    <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:1">
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f>_xlfn.SWITCH(B12,"Trace","T","Debug","D","Information","I","Warning","W","Error","E","Exception","X")</f>
+        <v>X</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>"PL"&amp;C12&amp;RIGHT("0000"&amp;A12,4)</f>
+        <v>PLX0011</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="4" t="str">
+        <f>D12&amp;": "&amp;E12</f>
+        <v>PLX0011: 参数 “{0}”超出了指定的范围。</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" customHeight="1" spans="1:1">
+      <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f>_xlfn.SWITCH(B13,"Trace","T","Debug","D","Information","I","Warning","W","Error","E","Exception","X")</f>
+        <v>X</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f>"PL"&amp;C13&amp;RIGHT("0000"&amp;A13,4)</f>
+        <v>PLX0012</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="4" t="str">
+        <f>D13&amp;": "&amp;E13</f>
+        <v>PLX0012: 参数 “{0}”超出了指定的范围 “{1}”。</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:6">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" customHeight="1" spans="1:1">
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3" t="str">
+        <f>_xlfn.SWITCH(B14,"Trace","T","Debug","D","Information","I","Warning","W","Error","E","Exception","X")</f>
+        <v>X</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f>"PL"&amp;C14&amp;RIGHT("0000"&amp;A14,4)</f>
+        <v>PLX0013</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="4" t="str">
+        <f>D14&amp;": "&amp;E14</f>
+        <v>PLX0013: 参数超出了指定的范围。</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:6">
       <c r="A15" s="2">
         <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f>_xlfn.SWITCH(B15,"Trace","T","Debug","D","Information","I","Warning","W","Error","E","Exception","X")</f>
+        <v>X</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f>"PL"&amp;C15&amp;RIGHT("0000"&amp;A15,4)</f>
+        <v>PLX0014</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="4" t="str">
+        <f>D15&amp;": "&amp;E15</f>
+        <v>PLX0014: 参数超出了指定的范围 “{0}”。</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:1">
@@ -1576,7 +1660,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9 B10:B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B12 B13 B2:B10 B14:B15">
       <formula1>"Trace,Debug,Information,Warning,Error,Exception"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>